<commit_message>
formatacao cond e linhas
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Formatacao/3.Formatacao_condicional.xlsx
+++ b/2.Excel/hands-on/5.Formatacao/3.Formatacao_condicional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Formatacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E58E0C-5858-4431-BFBD-4BE67E30AA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F735BBC-7AE4-4E02-9B4A-5190B1C1AF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11196" yWindow="0" windowWidth="12192" windowHeight="13056" firstSheet="3" activeTab="4" xr2:uid="{60DE4CDD-BFE8-488F-B25C-A1E3AA20DCD1}"/>
   </bookViews>
@@ -247,7 +247,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1001,20 +1022,20 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"Nacional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"Internacional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>100000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
       <formula>1000000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1307,11 +1328,11 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="top10" dxfId="4" priority="3" percent="1" rank="25"/>
-    <cfRule type="top10" dxfId="3" priority="2" percent="1" bottom="1" rank="25"/>
+    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="25"/>
+    <cfRule type="top10" dxfId="6" priority="2" percent="1" bottom="1" rank="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+    <cfRule type="aboveAverage" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1953,7 +1974,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2232,6 +2253,11 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="A2:D17">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$C2&gt;75000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>